<commit_message>
Update seller part backlog
</commit_message>
<xml_diff>
--- a/Doc/Sprint0/Product Backlog/Product BackLog_Seller Part.xlsx
+++ b/Doc/Sprint0/Product Backlog/Product BackLog_Seller Part.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98E96EE-2697-4C89-B457-CBDCAC0DB745}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6630684B-E218-4CE5-AAFB-6CDE13752753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>User Stories</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,7 +106,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>As a seller I should be able to report to admin</t>
+    <t>As a seller I should be able to report to admin about my questions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coding: Design and Implement admin contact page. Including question editing and commit.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coding: Implement Database access to admin question table.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding: Implement Database access to general account table, account validation, update account status.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding: Implement Database access to seller account table, update account status.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member in charge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yunwei Jiang
+Jingzhou Hu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -114,7 +141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +162,15 @@
       <name val="ArialMT"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -167,25 +203,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -466,169 +559,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="69.625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="77.25" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="10" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="42.75">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" ht="28.5" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="37.5" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="31.5" customHeight="1">
+      <c r="C5" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.5">
-      <c r="A7" s="4" t="s">
+      <c r="C8" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="29.25" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="28.5">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="28.5" customHeight="1">
+      <c r="C9" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="28.5">
-      <c r="A11" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" customHeight="1">
+      <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="28.5">
-      <c r="A13" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" customHeight="1">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="28.5">
-      <c r="A15" s="4" t="s">
-        <v>14</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" customHeight="1">
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>16</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.5">
-      <c r="A17" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" customHeight="1">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>17</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="28.5">
-      <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1">
+      <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="28.5">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>6</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" customHeight="1">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" customHeight="1">
       <c r="A22" s="4"/>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" customHeight="1">
+      <c r="A23" s="4"/>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C24" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
+  <mergeCells count="7">
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify seller backlog - Yunwei Jiang
</commit_message>
<xml_diff>
--- a/Doc/Sprint0/Product Backlog/Product BackLog_Seller Part.xlsx
+++ b/Doc/Sprint0/Product Backlog/Product BackLog_Seller Part.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6630684B-E218-4CE5-AAFB-6CDE13752753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3339A9BE-E172-4882-AAC7-4F9A2A4B6A7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>User Stories</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,15 +68,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>As a seller, I want to have Payment Gateway to sell the Goods .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Database Desgin: Payment table.
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>As a seller , I want display picture for my account and add details like name, Contact no. (Optional) for buyers to view and contact the seller.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -132,8 +123,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Yunwei Jiang
-Jingzhou Hu</t>
+    <t>Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status
+(0 = not started
+1 = working on
+2 = finished)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>As a seller, I want to have Payment Gateway to sell the Goods .</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Order</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -180,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -240,11 +245,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -253,31 +267,49 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,259 +591,323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="7" customWidth="1"/>
-    <col min="2" max="2" width="77.25" style="7" customWidth="1"/>
-    <col min="3" max="3" width="19" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.375" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="9" style="14"/>
+    <col min="2" max="2" width="20.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="77.25" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:6" s="10" customFormat="1" ht="60" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:6" ht="30" customHeight="1">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1">
+      <c r="A3" s="13"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" customHeight="1">
+      <c r="A4" s="13"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="1">
+      <c r="A5" s="13">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="1">
+      <c r="A6" s="13"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" customHeight="1">
+      <c r="A7" s="13"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" customHeight="1">
+      <c r="A8" s="13"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" customHeight="1">
+      <c r="A9" s="13">
+        <v>3</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1">
+      <c r="A10" s="13"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" customHeight="1">
+      <c r="A11" s="13"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" customHeight="1">
+      <c r="A12" s="13"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" customHeight="1">
+      <c r="A13" s="13">
+        <v>4</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" customHeight="1">
+      <c r="A14" s="13"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" customHeight="1">
+      <c r="A15" s="13"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" customHeight="1">
+      <c r="A16" s="13"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1">
+      <c r="A17" s="13">
+        <v>5</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1">
+      <c r="A18" s="13"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1">
+      <c r="A19" s="13"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1">
+      <c r="A20" s="13"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1">
+      <c r="A21" s="13">
+        <v>6</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1">
+      <c r="A23" s="13"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>26</v>
+      <c r="D23" s="4"/>
+      <c r="F23" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B21:B22"/>
+  <mergeCells count="13">
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A21:A23"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>